<commit_message>
Update Tag Reference Guide - v 1.0.1
</commit_message>
<xml_diff>
--- a/PHA4GE QC Tag Reference Guide.xlsx
+++ b/PHA4GE QC Tag Reference Guide.xlsx
@@ -1,27 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmagriffiths/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11639736-7C0D-F444-836A-296FE837B38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Field Reference Guide" sheetId="1" r:id="rId1"/>
-    <sheet name="Term Reference Guide" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="Field Reference Guide" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Term Reference Guide" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
   <si>
     <t>Parent Class</t>
   </si>
@@ -56,6 +47,9 @@
     <t>The name of the method used to assess whether a sequence passed a predetermined quality control threshold.</t>
   </si>
   <si>
+    <t>Providing the name of the method used for quality control is very important for interpreting the rest of the QC information. Method names can be provided as the name of a pipeline or a link to a GitHub repository. Multiple methods should be listed and separated by a semi-colon. Do not include QC tags in other fields if no method name is provided.</t>
+  </si>
+  <si>
     <t>ncov-tools</t>
   </si>
   <si>
@@ -68,6 +62,9 @@
     <t>The version number of the method used to assess whether a sequence passed a predetermined quality control threshold.</t>
   </si>
   <si>
+    <t>Methods updates can make big differences to their outputs. Provide the version of the method used for quality control. The version can be expressed using whatever convention the developer implements (e.g. date, semantic versioning). If multiple methods were used, record the version numbers in the same order as the method names. Separate the version numbers using a semi-colon.</t>
+  </si>
+  <si>
     <t>1.2.3</t>
   </si>
   <si>
@@ -80,6 +77,23 @@
     <t>The determination of a quality control assessment.</t>
   </si>
   <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Select a value from the pick list provided. If a desired value is missing, submit a new term request to the </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>PHA4GE QC Tag GitHub issuetracker using the New Term Request form.</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
     <t>sequence failed quality control [GENEPIO:0100564]</t>
   </si>
   <si>
@@ -92,6 +106,23 @@
     <t>The reason contributing to, or causing, a low quality determination in a quality control assessment.</t>
   </si>
   <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Select a value from the pick list provided. If a desired value is missing, </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>submit a new term request to the PHA4GE QC Tag GitHub issuetracker using the New Term Request form</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">.  </t>
+    </r>
+  </si>
+  <si>
     <t>low average genome coverage [GENEPIO:0100570]</t>
   </si>
   <si>
@@ -102,6 +133,9 @@
   </si>
   <si>
     <t>The details surrounding a low quality determination in a quality control assessment.</t>
+  </si>
+  <si>
+    <t>Provide notes or details regarding QC results using free text.</t>
   </si>
   <si>
     <t>CT value of 39. Low viral load. Low DNA concentration after amplification.</t>
@@ -305,73 +339,62 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="11">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -379,7 +402,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -395,60 +418,78 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="16">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -638,29 +679,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.5" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="40.6640625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="27.5"/>
+    <col customWidth="1" min="2" max="2" width="26.0"/>
+    <col customWidth="1" min="3" max="3" width="17.25"/>
+    <col customWidth="1" min="6" max="6" width="40.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,17 +736,17 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -728,120 +766,138 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+    <row r="3">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="F3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="E4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>27</v>
+      <c r="B7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E5"/>
+    <hyperlink r:id="rId2" ref="E6"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="103" customWidth="1"/>
-    <col min="5" max="5" width="65.1640625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="23.63"/>
+    <col customWidth="1" min="2" max="2" width="42.63"/>
+    <col customWidth="1" min="3" max="3" width="19.88"/>
+    <col customWidth="1" min="4" max="4" width="29.5"/>
+    <col customWidth="1" min="5" max="5" width="65.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -872,14 +928,14 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -900,18 +956,18 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -934,18 +990,18 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -968,20 +1024,19 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1002,18 +1057,18 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1036,18 +1091,18 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1070,14 +1125,14 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8">
       <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1098,116 +1153,116 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="10" t="s">
+    <row r="9">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="C9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="E9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="10" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="C10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="E10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="10" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="C11" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="E11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="11" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="C12" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="10" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="C13" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E13" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1228,122 +1283,122 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="7" t="s">
+    <row r="16">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D16" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="7" t="s">
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="12" t="s">
+      <c r="C17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="7" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="12" t="s">
+      <c r="C18" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="D18" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="7" t="s">
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="12" t="s">
+      <c r="C19" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="D19" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="7" t="s">
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="12" t="s">
+      <c r="C20" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="D20" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="7" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="12" t="s">
+      <c r="C21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="D21" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="7" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>92</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D5:E5"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>